<commit_message>
updated status info and added cc to the accepted/rejected notification emails
</commit_message>
<xml_diff>
--- a/Scanorders2/src/Oleg/FellAppBundle/Util/GoogleForm/FellowshipRecommendationLetters/TemplateSpreadsheet.xlsx
+++ b/Scanorders2/src/Oleg/FellAppBundle/Util/GoogleForm/FellowshipRecommendationLetters/TemplateSpreadsheet.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId3"/>
@@ -199,11 +199,11 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>